<commit_message>
Minor updates to work with chart program
</commit_message>
<xml_diff>
--- a/Test Case - 7/TC7_Results_B.xlsx
+++ b/Test Case - 7/TC7_Results_B.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -743,19 +743,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -802,7 +802,27 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -905,16 +925,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -945,11 +955,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1252,7 +1262,7 @@
   <dimension ref="A1:R63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+      <selection activeCell="O51" sqref="O51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,20 +1271,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="5" t="s">
         <v>67</v>
       </c>
       <c r="I1" s="4" t="s">
@@ -1289,7 +1299,7 @@
       <c r="L1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="5" t="s">
         <v>72</v>
       </c>
       <c r="N1" s="4" t="s">
@@ -1298,43 +1308,43 @@
       <c r="O1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="2"/>
+      <c r="H2" s="5"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="2"/>
+      <c r="M2" s="5"/>
       <c r="N2" s="4" t="s">
         <v>73</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -2957,6 +2967,9 @@
       </c>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
+      <c r="Q34" t="b">
+        <v>1</v>
+      </c>
       <c r="R34" t="s">
         <v>34</v>
       </c>
@@ -3001,6 +3014,9 @@
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
+      <c r="Q35" t="b">
+        <v>1</v>
+      </c>
       <c r="R35" t="s">
         <v>34</v>
       </c>
@@ -3045,6 +3061,9 @@
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
+      <c r="Q36" t="b">
+        <v>1</v>
+      </c>
       <c r="R36" t="s">
         <v>34</v>
       </c>
@@ -3089,6 +3108,9 @@
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
+      <c r="Q37" t="b">
+        <v>1</v>
+      </c>
       <c r="R37" t="s">
         <v>34</v>
       </c>
@@ -3133,6 +3155,9 @@
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
+      <c r="Q38" t="b">
+        <v>1</v>
+      </c>
       <c r="R38" t="s">
         <v>34</v>
       </c>
@@ -3177,6 +3202,9 @@
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
+      <c r="Q39" t="b">
+        <v>1</v>
+      </c>
       <c r="R39" t="s">
         <v>34</v>
       </c>
@@ -3221,6 +3249,9 @@
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
+      <c r="Q40" t="b">
+        <v>1</v>
+      </c>
       <c r="R40" t="s">
         <v>34</v>
       </c>
@@ -3265,6 +3296,9 @@
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
+      <c r="Q41" t="b">
+        <v>1</v>
+      </c>
       <c r="R41" t="s">
         <v>34</v>
       </c>
@@ -3309,6 +3343,9 @@
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
+      <c r="Q42" t="b">
+        <v>1</v>
+      </c>
       <c r="R42" t="s">
         <v>34</v>
       </c>
@@ -3353,6 +3390,9 @@
       <c r="M43" s="4"/>
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
+      <c r="Q43" t="b">
+        <v>1</v>
+      </c>
       <c r="R43" t="s">
         <v>34</v>
       </c>
@@ -3397,6 +3437,9 @@
       <c r="M44" s="4"/>
       <c r="N44" s="4"/>
       <c r="O44" s="4"/>
+      <c r="Q44" t="b">
+        <v>1</v>
+      </c>
       <c r="R44" t="s">
         <v>34</v>
       </c>
@@ -3441,6 +3484,9 @@
       <c r="M45" s="4"/>
       <c r="N45" s="4"/>
       <c r="O45" s="4"/>
+      <c r="Q45" t="b">
+        <v>1</v>
+      </c>
       <c r="R45" t="s">
         <v>34</v>
       </c>
@@ -4179,6 +4225,10 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:H2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="M34:O45"/>
@@ -4187,36 +4237,40 @@
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="L3:L63">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q7">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q13:Q14">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q16">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q17">
     <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -4224,7 +4278,7 @@
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q17">
+  <conditionalFormatting sqref="Q22">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -4232,7 +4286,7 @@
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q22">
+  <conditionalFormatting sqref="Q25">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -4240,7 +4294,7 @@
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q25">
+  <conditionalFormatting sqref="Q28">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
@@ -4248,11 +4302,11 @@
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q28">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="Q34:Q45">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>